<commit_message>
Updated training data structure used for bracket models
</commit_message>
<xml_diff>
--- a/kentucky.xlsx
+++ b/kentucky.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23801"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -10,7 +10,7 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="100" documentId="11_FFC65FC04469ACD3AE160BB8A37FBEBD68106C17" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{3209B3AC-2392-4925-8C04-835F0EF0DEAF}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView minimized="1" xWindow="-25080" yWindow="3720" windowWidth="21600" windowHeight="11325" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -907,8 +907,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:CI16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AN1" workbookViewId="0">
-      <selection activeCell="AO2" sqref="AO2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>